<commit_message>
Refactor generate_daily_schedule.py to validate file type and headers, and add error handling
</commit_message>
<xml_diff>
--- a/test_data_daily_schedule.xlsx
+++ b/test_data_daily_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angga\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_fastapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068E1162-F931-4450-A2EE-D6F81D39CF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B451C83E-0D15-406E-93AC-93FDD66A0C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D510C39D-273F-454A-9CB1-C78D5EE15B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1102,9 +1100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1142,7 +1140,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1248,7 +1246,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1390,7 +1388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1400,15 +1398,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244F6AE9-728D-E247-A126-31EDB904D4D8}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E35" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H51"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.296875" customWidth="1"/>
-    <col min="5" max="5" width="60.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="73.296875" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+    <col min="5" max="5" width="60.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="73.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">

</xml_diff>